<commit_message>
Update input files, working parameters file
</commit_message>
<xml_diff>
--- a/antha/component/an/Liquid_handling/PooledLibrary/playground/Rewiringinput2.xlsx
+++ b/antha/component/an/Liquid_handling/PooledLibrary/playground/Rewiringinput2.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26709"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/theukshowdown/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="8200" tabRatio="990"/>
+    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="14940" tabRatio="990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="45">
   <si>
     <t>Run</t>
   </si>
@@ -159,9 +154,6 @@
   </si>
   <si>
     <t>rpoN</t>
-  </si>
-  <si>
-    <t>PhoA</t>
   </si>
   <si>
     <t>ihfA_B</t>
@@ -201,7 +193,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -209,15 +201,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
@@ -344,7 +416,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic Light"/>
@@ -379,7 +451,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="Yu Gothic"/>
@@ -556,7 +628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -564,15 +636,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B9" sqref="B9:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -589,12 +661,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
-        <v>121</v>
+      <c r="B2" s="3">
+        <v>34.18</v>
       </c>
       <c r="C2">
         <v>855</v>
@@ -606,12 +678,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
-        <v>202</v>
+      <c r="B3" s="4">
+        <v>71.510000000000005</v>
       </c>
       <c r="C3">
         <v>993</v>
@@ -623,12 +695,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4">
-        <v>81</v>
+      <c r="B4" s="4">
+        <v>90.64</v>
       </c>
       <c r="C4">
         <v>879</v>
@@ -640,12 +712,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>358</v>
+      <c r="B5" s="4">
+        <v>140.97999999999999</v>
       </c>
       <c r="C5">
         <v>2706</v>
@@ -657,12 +729,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>300</v>
+      <c r="B6" s="4">
+        <v>559.83000000000004</v>
       </c>
       <c r="C6">
         <v>744</v>
@@ -671,15 +743,15 @@
         <v>2709</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7">
-        <v>270</v>
+      <c r="B7" s="4">
+        <v>256.49</v>
       </c>
       <c r="C7">
         <v>717</v>
@@ -691,12 +763,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8">
-        <v>176</v>
+      <c r="B8" s="4">
+        <v>336.86</v>
       </c>
       <c r="C8">
         <v>750</v>
@@ -708,12 +780,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9">
-        <v>228</v>
+      <c r="B9" s="6">
+        <v>72.2</v>
       </c>
       <c r="C9" s="2">
         <v>297</v>
@@ -725,12 +797,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10">
-        <v>225</v>
+      <c r="B10" s="7">
+        <v>77.400000000000006</v>
       </c>
       <c r="C10">
         <v>753</v>
@@ -742,12 +814,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>14</v>
       </c>
-      <c r="B11">
-        <v>87</v>
+      <c r="B11" s="7">
+        <v>86.06</v>
       </c>
       <c r="C11">
         <v>576</v>
@@ -759,12 +831,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
-      <c r="B12">
-        <v>283</v>
+      <c r="B12" s="7">
+        <v>56.56</v>
       </c>
       <c r="C12">
         <v>414</v>
@@ -776,12 +848,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13">
-        <v>274</v>
+      <c r="B13" s="7">
+        <v>203.01</v>
       </c>
       <c r="C13">
         <v>633</v>
@@ -793,12 +865,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>17</v>
       </c>
-      <c r="B14">
-        <v>200</v>
+      <c r="B14" s="7">
+        <v>382.3</v>
       </c>
       <c r="C14">
         <v>720</v>
@@ -810,12 +882,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>18</v>
       </c>
-      <c r="B15">
-        <v>193</v>
+      <c r="B15" s="7">
+        <v>75.349999999999994</v>
       </c>
       <c r="C15">
         <v>932</v>
@@ -827,12 +899,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B16">
-        <v>85</v>
+      <c r="B16" s="8">
+        <v>228.31</v>
       </c>
       <c r="C16">
         <v>1842</v>
@@ -844,12 +916,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>20</v>
       </c>
-      <c r="B17">
-        <v>77</v>
+      <c r="B17" s="3">
+        <v>87.99</v>
       </c>
       <c r="C17">
         <v>495</v>
@@ -861,12 +933,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18">
-        <v>171</v>
+      <c r="B18" s="4">
+        <v>88.67</v>
       </c>
       <c r="C18" s="2">
         <v>163</v>
@@ -878,12 +950,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>22</v>
       </c>
-      <c r="B19">
-        <v>253</v>
+      <c r="B19" s="4">
+        <v>432.29</v>
       </c>
       <c r="C19">
         <v>723</v>
@@ -895,12 +967,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>23</v>
       </c>
-      <c r="B20">
-        <v>382</v>
+      <c r="B20" s="4">
+        <v>87.19</v>
       </c>
       <c r="C20">
         <v>651</v>
@@ -912,12 +984,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-      <c r="B21">
-        <v>260</v>
+      <c r="B21" s="4">
+        <v>170.69</v>
       </c>
       <c r="C21">
         <v>699</v>
@@ -929,12 +1001,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>25</v>
       </c>
-      <c r="B22">
-        <v>207</v>
+      <c r="B22" s="4">
+        <v>281.83999999999997</v>
       </c>
       <c r="C22">
         <v>705</v>
@@ -946,12 +1018,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>26</v>
       </c>
-      <c r="B23">
-        <v>192</v>
+      <c r="B23" s="4">
+        <v>58.97</v>
       </c>
       <c r="C23">
         <v>723</v>
@@ -963,12 +1035,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>27</v>
       </c>
-      <c r="B24">
-        <v>72</v>
+      <c r="B24" s="5">
+        <v>134.66999999999999</v>
       </c>
       <c r="C24">
         <v>900</v>
@@ -980,12 +1052,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-      <c r="B25">
-        <v>90</v>
+      <c r="B25" s="6">
+        <v>239.77</v>
       </c>
       <c r="C25">
         <v>762</v>
@@ -997,12 +1069,12 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>29</v>
       </c>
-      <c r="B26">
-        <v>302</v>
+      <c r="B26" s="7">
+        <v>179.01</v>
       </c>
       <c r="C26">
         <v>720</v>
@@ -1014,12 +1086,12 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>30</v>
       </c>
-      <c r="B27">
-        <v>358</v>
+      <c r="B27" s="7">
+        <v>164.07</v>
       </c>
       <c r="C27">
         <v>624</v>
@@ -1031,12 +1103,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>31</v>
       </c>
-      <c r="B28">
-        <v>314</v>
+      <c r="B28" s="7">
+        <v>398.97</v>
       </c>
       <c r="C28">
         <v>1260</v>
@@ -1048,12 +1120,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>32</v>
       </c>
-      <c r="B29">
-        <v>320</v>
+      <c r="B29" s="7">
+        <v>122.47</v>
       </c>
       <c r="C29" s="2">
         <v>318</v>
@@ -1065,12 +1137,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>33</v>
       </c>
-      <c r="B30">
-        <v>212</v>
+      <c r="B30" s="7">
+        <v>326.42</v>
       </c>
       <c r="C30">
         <v>720</v>
@@ -1082,12 +1154,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>34</v>
       </c>
-      <c r="B31">
-        <v>202</v>
+      <c r="B31" s="7">
+        <v>39.61</v>
       </c>
       <c r="C31" s="2">
         <v>267</v>
@@ -1099,12 +1171,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>35</v>
       </c>
-      <c r="B32">
-        <v>74</v>
+      <c r="B32" s="8">
+        <v>171.28</v>
       </c>
       <c r="C32">
         <v>537</v>
@@ -1116,12 +1188,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>36</v>
       </c>
-      <c r="B33">
-        <v>100</v>
+      <c r="B33" s="3">
+        <v>222.18</v>
       </c>
       <c r="C33">
         <v>477</v>
@@ -1133,12 +1205,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>37</v>
       </c>
-      <c r="B34">
-        <v>185</v>
+      <c r="B34" s="4">
+        <v>145.12</v>
       </c>
       <c r="C34">
         <v>477</v>
@@ -1150,12 +1222,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>38</v>
       </c>
-      <c r="B35">
-        <v>283</v>
+      <c r="B35" s="4">
+        <v>253.1</v>
       </c>
       <c r="C35">
         <v>621</v>
@@ -1167,12 +1239,12 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>39</v>
       </c>
-      <c r="B36">
-        <v>301</v>
+      <c r="B36" s="4">
+        <v>247.02</v>
       </c>
       <c r="C36">
         <v>918</v>
@@ -1184,12 +1256,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>40</v>
       </c>
-      <c r="B37">
-        <v>296</v>
+      <c r="B37" s="4">
+        <v>37.56</v>
       </c>
       <c r="C37">
         <v>825</v>
@@ -1201,12 +1273,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>41</v>
       </c>
-      <c r="B38">
-        <v>216</v>
+      <c r="B38" s="4">
+        <v>250</v>
       </c>
       <c r="C38">
         <v>402</v>
@@ -1218,12 +1290,12 @@
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>42</v>
       </c>
-      <c r="B39">
-        <v>225</v>
+      <c r="B39" s="4">
+        <v>281.18</v>
       </c>
       <c r="C39" s="2">
         <v>219</v>
@@ -1235,12 +1307,12 @@
         <v>42</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>43</v>
       </c>
-      <c r="B40">
-        <v>65</v>
+      <c r="B40" s="5">
+        <v>36.090000000000003</v>
       </c>
       <c r="C40">
         <v>1434</v>
@@ -1250,27 +1322,15 @@
       </c>
       <c r="E40" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41">
-        <v>100</v>
-      </c>
-      <c r="C41">
-        <v>1416</v>
-      </c>
-      <c r="D41">
-        <v>4130</v>
-      </c>
-      <c r="E41" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>